<commit_message>
add negative power to see whether it works + add run.bat
</commit_message>
<xml_diff>
--- a/busIn.xlsx
+++ b/busIn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GITHUB_PRIVATE_CODES\ForwardBackwardSweep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E4E787-27FE-43FA-905E-3BC6D00B8ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C762A718-3682-4775-8123-AFCF70F828C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4FDC1957-8DB4-4927-B139-8B72076C7FCA}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>120</v>
       </c>
       <c r="B5">
-        <v>80</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>200</v>
+        <v>-200</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>420</v>
+        <v>-420</v>
       </c>
       <c r="B26">
         <v>200</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>60</v>
+        <v>-60</v>
       </c>
       <c r="B28">
         <v>25</v>
@@ -647,7 +647,7 @@
         <v>200</v>
       </c>
       <c r="B31">
-        <v>600</v>
+        <v>-600</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>